<commit_message>
Included new observers in observer_ids.csv and observer_ids.xlsx.
</commit_message>
<xml_diff>
--- a/colordeficiency-data/observer_ids.xlsx
+++ b/colordeficiency-data/observer_ids.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="12460" yWindow="960" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>HM</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>BO</t>
+  </si>
+  <si>
+    <t>OM</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>ZS</t>
   </si>
 </sst>
 </file>
@@ -452,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.83203125" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0"/>
@@ -750,6 +759,39 @@
       </c>
       <c r="C26" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="23.25" customHeight="1">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="23.25" customHeight="1">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="23.25" customHeight="1">
+      <c r="A29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
settings: Changed yoshi-gradient to yoshi-ii. - colordeficiency_tools: Added getColDefTypeForObserver. - analysis_tools: Change filenames for chi2 test, median test, student-t test. - analysis: Filter by observer group and coldef_type in visdemPlots53Thru60 and makePairedDataForViSDEM. - Added new observer_ids.
</commit_message>
<xml_diff>
--- a/colordeficiency-data/observer_ids.xlsx
+++ b/colordeficiency-data/observer_ids.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>observer_id</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>GW</t>
+  </si>
+  <si>
+    <t>CL</t>
   </si>
 </sst>
 </file>
@@ -959,21 +962,31 @@
       <c r="B51" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C51" s="2"/>
+      <c r="C51" s="2">
+        <v>2.0</v>
+      </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
     </row>
     <row r="52" ht="23.25" customHeight="1">
-      <c r="A52" s="2"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="2"/>
+      <c r="A52" s="2">
+        <v>51.0</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" s="2">
+        <v>2.0</v>
+      </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
     </row>
     <row r="53" ht="23.25" customHeight="1">
-      <c r="A53" s="2"/>
+      <c r="A53" s="2">
+        <v>52.0</v>
+      </c>
       <c r="B53" s="1"/>
       <c r="C53" s="2"/>
       <c r="D53" s="1"/>
@@ -981,7 +994,9 @@
       <c r="F53" s="1"/>
     </row>
     <row r="54" ht="23.25" customHeight="1">
-      <c r="A54" s="2"/>
+      <c r="A54" s="2">
+        <v>53.0</v>
+      </c>
       <c r="B54" s="1"/>
       <c r="C54" s="2"/>
       <c r="D54" s="1"/>
@@ -989,7 +1004,9 @@
       <c r="F54" s="1"/>
     </row>
     <row r="55" ht="23.25" customHeight="1">
-      <c r="A55" s="2"/>
+      <c r="A55" s="2">
+        <v>54.0</v>
+      </c>
       <c r="B55" s="1"/>
       <c r="C55" s="2"/>
       <c r="D55" s="1"/>

</xml_diff>